<commit_message>
some citations filled in
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="1480" windowWidth="25600" windowHeight="12420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Leeds</t>
   </si>
@@ -30,34 +30,94 @@
     <t>Strathclyde</t>
   </si>
   <si>
-    <t>Years</t>
-  </si>
-  <si>
-    <t>WP1: Semantics</t>
-  </si>
-  <si>
-    <t>WP2: Type Theory</t>
-  </si>
-  <si>
-    <t>WP3: HITs</t>
-  </si>
-  <si>
-    <t>WP4: Effects</t>
-  </si>
-  <si>
-    <t>WP5: Metelanguage</t>
-  </si>
-  <si>
-    <t>WP6: Core</t>
-  </si>
-  <si>
-    <t>WP7: High Level Language</t>
-  </si>
-  <si>
-    <t>WP8: Case Studies</t>
-  </si>
-  <si>
     <t>Legend:</t>
+  </si>
+  <si>
+    <t>WP1</t>
+  </si>
+  <si>
+    <t>WP2</t>
+  </si>
+  <si>
+    <t>WP3</t>
+  </si>
+  <si>
+    <t>WP4</t>
+  </si>
+  <si>
+    <t>WP5</t>
+  </si>
+  <si>
+    <t>WP6</t>
+  </si>
+  <si>
+    <t>WP7</t>
+  </si>
+  <si>
+    <t>WP8</t>
+  </si>
+  <si>
+    <t>Year 1</t>
+  </si>
+  <si>
+    <t>Year 2</t>
+  </si>
+  <si>
+    <t>Year 3</t>
+  </si>
+  <si>
+    <t>Year 4</t>
+  </si>
+  <si>
+    <t>Workpackages:</t>
+  </si>
+  <si>
+    <t>WP1:</t>
+  </si>
+  <si>
+    <t>Semantic Foundations of HoTT</t>
+  </si>
+  <si>
+    <t>WP2:</t>
+  </si>
+  <si>
+    <t>Univalent Type Theory</t>
+  </si>
+  <si>
+    <t>WP3:</t>
+  </si>
+  <si>
+    <t>Higher Inductive Types.</t>
+  </si>
+  <si>
+    <t>WP4:</t>
+  </si>
+  <si>
+    <t>Impact I - Programming with Effects</t>
+  </si>
+  <si>
+    <t>WP5:</t>
+  </si>
+  <si>
+    <t>Formalisation of Meta-Theory of HoTT</t>
+  </si>
+  <si>
+    <t>WP6:</t>
+  </si>
+  <si>
+    <t>Implementing a Core Programming Language</t>
+  </si>
+  <si>
+    <t>WP7:</t>
+  </si>
+  <si>
+    <t>A High Level Programming Language</t>
+  </si>
+  <si>
+    <t>WP8:</t>
+  </si>
+  <si>
+    <t>Impact II - Programming and Invariance</t>
   </si>
 </sst>
 </file>
@@ -108,28 +168,22 @@
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
-      <patternFill patternType="darkUp">
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="darkDown">
-        <bgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
         <fgColor indexed="65"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="darkVertical">
-        <bgColor theme="7"/>
-      </patternFill>
+      <patternFill patternType="darkUp"/>
+    </fill>
+    <fill>
+      <patternFill patternType="darkDown"/>
+    </fill>
+    <fill>
+      <patternFill patternType="darkVertical"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -190,15 +244,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -231,7 +276,53 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
         <color auto="1"/>
       </right>
       <top/>
@@ -241,13 +332,9 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
+      <left/>
+      <right/>
+      <top style="thin">
         <color auto="1"/>
       </top>
       <bottom/>
@@ -255,29 +342,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top/>
       <bottom style="thin">
         <color auto="1"/>
@@ -285,7 +350,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -293,8 +358,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -302,41 +375,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -346,14 +389,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -683,234 +773,329 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection sqref="A1:E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
+      <c r="A1" s="41"/>
+      <c r="B1" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="16" thickBot="1">
-      <c r="A2" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="31"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="2"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="10"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="31"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="1"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="31"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="21"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="17"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="16" thickBot="1">
-      <c r="A7" s="31"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="31"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="31"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="21"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="31"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="9"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="22"/>
+      <c r="E11" s="27"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="31"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="21"/>
+      <c r="E12" s="28"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="31"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="16"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="1"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="31"/>
-      <c r="B15" s="13"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="2"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="31"/>
-      <c r="B16" s="14"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="3"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="27"/>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="31"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="31"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="8"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="20"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="33"/>
+      <c r="A21" s="13"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="13"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="23"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="34"/>
+      <c r="A22" s="14"/>
       <c r="C22" s="3"/>
-      <c r="E22" s="14"/>
+      <c r="E22" s="21"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="23"/>
+      <c r="E23" s="32"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="33"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="11"/>
+      <c r="E24" s="25"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="34"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="12"/>
+      <c r="E25" s="26"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="25"/>
+      <c r="A27" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="9"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="26"/>
-      <c r="B28" s="27" t="s">
+      <c r="A28" s="33"/>
+      <c r="B28" s="10" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="28"/>
-      <c r="B29" s="27" t="s">
+      <c r="A29" s="34"/>
+      <c r="B29" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="29"/>
-      <c r="B30" s="30" t="s">
+      <c r="A30" s="35"/>
+      <c r="B30" s="11" t="s">
         <v>2</v>
       </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="9"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="10"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="10"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="10"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="10"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="10"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="10"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="10"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -928,7 +1113,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>